<commit_message>
deleted testset data and faiss db content
</commit_message>
<xml_diff>
--- a/evaluate/testset.xlsx
+++ b/evaluate/testset.xlsx
@@ -1,37 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b440c95ba6615302/Dokumente/GitHub/CLLeMens/evaluate/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_67FD66929E52220F62355476585DCE3A87476A28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B62A8F0-38D7-4CAD-BEE2-A99446108BAA}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="9600" yWindow="3000" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Contexts</t>
+  </si>
+  <si>
+    <t>Ground Truth</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +69,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,83 +393,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Question</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Answer</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Contexts</t>
-        </is>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Ground Truth</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Who was the author of Masterarbeit Expose?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>The author of the Masterarbeit Expose is Alpay-Kaan Erbay.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>['Expos´ e f ¨ur eine Masterarbeit zum Thema:\nEinsatz maschineller Lernverfahren zur Bestimmung\nkritischer SEO-Parameter\nAlpay-Kaan Erbay\nHochschule Ruhr West, L ¨utzowstr. 5, Bottrop 46246, Deutschland\n25. M ¨arz 2024\n1', 'ohne eine tiefgehende Untersuchung der spezifischen Gewichtungen von Websei-\ntenparametern. Diese Arbeiten bieten wertvolle Einblicke in die Potenziale von\nmaschinellem Lernen f ¨ur SEO, lassen jedoch eine detaillierte Analyse dar ¨uber\nvermissen, nach welchen genauen Kriterien Google Webseiten bewertet und ein-\nstuft. Die vorliegende Arbeit erkennt diese Forschungsl ¨ucke und strebt danach,\nsie zu schließen, indem sie ein maßgeschneidertes neuronales Netz entwickelt,\nwelches speziell darauf ausgerichtet ist, die Gewichtungen und Interaktionen\nverschiedener SEO-relevanter Parameter im Ranking-Algorithmus von Google', 'zu entschl ¨usseln. Dadurch soll nicht nur das Verst ¨andnis der Funktionsweise\nvon Googles Algorithmus vertieft, sondern auch konkrete Hinweise darauf ge-\nliefert werden, welche Aspekte von Webseiten f ¨ur eine optimale Positionierung\nin den Suchergebnissen entscheidend sind. Diese spezifische Ausrichtung auf die\nAnalyse der Parametergewichtungen unterscheidet die vorliegende Arbeit deut-\nlich von bisherigen Ans ¨atzen und verspricht, pr ¨azisere und anwendungsbezogene\nErkenntnisse f ¨ur die Optimierung von Webseiten zu liefern.\n4 Methodik\nDie vorliegende Arbeit verfolgt die zentrale Fragestellung, ob es m ¨oglich ist,', '5 Erwartete Ergebnisse\nEs wird erwartet, dass die Arbeit signifikante neue Erkenntnisse dar ¨uber liefert,\nwelche Faktoren f ¨ur Google-Rankings entscheidend sind und wie diese inter-\nagieren. Das entwickelte Modell soll nicht nur aktuelle Einblicke in die Algo-\nrithmen von Google bieten, sondern auch die F ¨ahigkeit besitzen, sich an deren\nkontinuierliche ¨Anderungen anzupassen, um stets relevante und zeitnahe SEO-\nEmpfehlungen zu erm ¨oglichen. Damit leistet die Arbeit einen bedeutenden Bei-\ntrag zur SEO-Forschung und -Praxis.\nLiteratur\n[1] Indriyatmoko, T., Rahardi, M.: Relevansi Search Engine Optimization\n(SEO) On-pages Di 2021. Jurnal Ilmiah Komputer dan Bisnis 2(1),', 'und Unternehmen erm ¨oglicht, ihre Sichtbarkeit im digitalen Raum strategisch\nzu ver-bessern.\n2 Zielsetzung und Erkenntnisinteresse\nZiel dieser Arbeit ist es, durch die Entwicklung eines spezialisierten neuronalen\nNetzwerks tiefere Einblicke in die Funktionsweise von Googles Ranking-Algo-\nrithmen zu gewinnen. Das Erkenntnisinteresse liegt insbesondere darin, zu ver-\nstehen, welche Parameter von Google bevorzugt werden und wie diese das Ran-\nking beeinflussen, um darauf aufbauend pr ¨azise Vorhersagen ¨uber das Ranking\nvon Webseiten unter Ber ¨ucksichtigung einer breiten Palette von Parametern zu\nerm¨oglichen.\n3 Forschungsstand und theoretische Grundlagen', 'Eine weitere Studie untersucht die Anwendung von maschinellem Lernen, ins-\nbesondere des Graph Neural Network (GNN), auf das Ranking von Webseiten.\n3', 'Ziel ist es, zu zeigen, dass GNN verschiedene existierende Ranking-Methoden wie\nPageRank, TrustRank, HITS und OPIC lernen und anwenden kann. Dadurch\nsoll eine flexiblere und m ¨oglicherweise effizientere Methode zur Bewertung und\nEinordnung von Webseiten im Kontext der Suchmaschinenoptimierung etabliert\nwerden. Dabei wird auf die Analyse von Netzwerkstrukturen und Beziehungen\nzwischen Webseite gesetzt (Yong et al., 2008).\nForschungsl ¨ucke und Beitrag dieser Arbeit:\nW¨ahrend bereits einige Forschungsarbeiten den Einsatz neuronaler Netze zur\nAnalyse und Verbesserung von Google-Rankings erforscht haben, fokussieren\nsich diese meist auf die allgemeine Anwendung maschinellen Lernens in der SEO', 'regeln der Suchmaschinenoptimierung regelm ¨aßig ver ¨andern. Entwickler und\nSEO-Experten stehen somit vor der schwierigen Aufgabe, ohne klare Einsicht\nin die spezifischen Gewichtungen und Interaktionen der Ranking-Faktoren eine\neffektive SEO-Strategie zu entwickeln. Die Dynamik der Suchmaschinenopti-\nmierung (SEO) ist somit maßgeblich von den undurchsichtigen Algorithmen\nder Suchmaschinen, insbesondere Google, gepr ¨agt. Die zentrale Herausforde-\nrung besteht darin, diese komplexen und oft intransparenten Mechanismen zu\nent-schl ¨usseln, um eine SEO-Strategie zu entwickeln und kontinuierlich anzu-\npassen, die den st ¨andig wechselnden Anforderungen von Google gerecht wird']</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>The Author is Alpay-Kaan Erbay</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>What is the Masterarbeit Expose about?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>The Masterarbeit Expose is about using machine learning methods to determine critical SEO parameters. The aim of the work is to gain deeper insights into Google's ranking algorithms through the development of a specialized neural network. The goal is to understand which parameters Google prefers and how these influence the ranking. Based on this, the work seeks to make precise predictions about the ranking of websites, considering a wide range of parameters. The research aims to fill a knowledge gap in understanding how Google evaluates and ranks websites based on specific parameters. The work expects to provide significant new insights into what factors are crucial for Google rankings and how they interact.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>['Expos´ e f ¨ur eine Masterarbeit zum Thema:\nEinsatz maschineller Lernverfahren zur Bestimmung\nkritischer SEO-Parameter\nAlpay-Kaan Erbay\nHochschule Ruhr West, L ¨utzowstr. 5, Bottrop 46246, Deutschland\n25. M ¨arz 2024\n1', 'und Unternehmen erm ¨oglicht, ihre Sichtbarkeit im digitalen Raum strategisch\nzu ver-bessern.\n2 Zielsetzung und Erkenntnisinteresse\nZiel dieser Arbeit ist es, durch die Entwicklung eines spezialisierten neuronalen\nNetzwerks tiefere Einblicke in die Funktionsweise von Googles Ranking-Algo-\nrithmen zu gewinnen. Das Erkenntnisinteresse liegt insbesondere darin, zu ver-\nstehen, welche Parameter von Google bevorzugt werden und wie diese das Ran-\nking beeinflussen, um darauf aufbauend pr ¨azise Vorhersagen ¨uber das Ranking\nvon Webseiten unter Ber ¨ucksichtigung einer breiten Palette von Parametern zu\nerm¨oglichen.\n3 Forschungsstand und theoretische Grundlagen', 'zu entschl ¨usseln. Dadurch soll nicht nur das Verst ¨andnis der Funktionsweise\nvon Googles Algorithmus vertieft, sondern auch konkrete Hinweise darauf ge-\nliefert werden, welche Aspekte von Webseiten f ¨ur eine optimale Positionierung\nin den Suchergebnissen entscheidend sind. Diese spezifische Ausrichtung auf die\nAnalyse der Parametergewichtungen unterscheidet die vorliegende Arbeit deut-\nlich von bisherigen Ans ¨atzen und verspricht, pr ¨azisere und anwendungsbezogene\nErkenntnisse f ¨ur die Optimierung von Webseiten zu liefern.\n4 Methodik\nDie vorliegende Arbeit verfolgt die zentrale Fragestellung, ob es m ¨oglich ist,', 'ohne eine tiefgehende Untersuchung der spezifischen Gewichtungen von Websei-\ntenparametern. Diese Arbeiten bieten wertvolle Einblicke in die Potenziale von\nmaschinellem Lernen f ¨ur SEO, lassen jedoch eine detaillierte Analyse dar ¨uber\nvermissen, nach welchen genauen Kriterien Google Webseiten bewertet und ein-\nstuft. Die vorliegende Arbeit erkennt diese Forschungsl ¨ucke und strebt danach,\nsie zu schließen, indem sie ein maßgeschneidertes neuronales Netz entwickelt,\nwelches speziell darauf ausgerichtet ist, die Gewichtungen und Interaktionen\nverschiedener SEO-relevanter Parameter im Ranking-Algorithmus von Google', '5 Erwartete Ergebnisse\nEs wird erwartet, dass die Arbeit signifikante neue Erkenntnisse dar ¨uber liefert,\nwelche Faktoren f ¨ur Google-Rankings entscheidend sind und wie diese inter-\nagieren. Das entwickelte Modell soll nicht nur aktuelle Einblicke in die Algo-\nrithmen von Google bieten, sondern auch die F ¨ahigkeit besitzen, sich an deren\nkontinuierliche ¨Anderungen anzupassen, um stets relevante und zeitnahe SEO-\nEmpfehlungen zu erm ¨oglichen. Damit leistet die Arbeit einen bedeutenden Bei-\ntrag zur SEO-Forschung und -Praxis.\nLiteratur\n[1] Indriyatmoko, T., Rahardi, M.: Relevansi Search Engine Optimization\n(SEO) On-pages Di 2021. Jurnal Ilmiah Komputer dan Bisnis 2(1),', 'Eine weitere Studie untersucht die Anwendung von maschinellem Lernen, ins-\nbesondere des Graph Neural Network (GNN), auf das Ranking von Webseiten.\n3', 'herangezogen. Durch den Vergleich dieser Metriken ¨uber die verschiedenen Mo-\ndelle hinweg k ¨onnen R ¨uckschl ¨usse auf die St ¨arken und Schw ¨achen der einzel-\nnen Ans ¨atze gezogen werden. Des Weiteren werden Sensitivit ¨atsanalysen durch-\ngef¨uhrt, um zu untersuchen, wie Ver ¨anderungen in den Daten oder Parametern\ndie Feature-Wichtigkeitsbewertungen beeinflussen. Diese systematische Bewer-\ntung erm ¨oglicht es, die Methoden objektiv zu vergleichen und diejenigen aus-\nzuw¨ahlen, die die zuverl ¨assigsten und aussagekr ¨aftigsten Einblicke in die Ge-\nwichtung der SEO-Parameter liefern.\n6', 'Raum erlernt wird. Dies ist n ¨utzlich, um die zugrundeliegende Struktur\nder Daten zu verstehen und die wichtigsten Features zu identifizieren, die\nf¨ur das Ranking einer Webseite ausschlaggebend sind. Die Reduktion auf\neinen latenten Raum erm ¨oglicht es, die komplexen Beziehungen zwischen\nden Features zu entwirren und diejenigen hervorzuheben, die f ¨ur die Vor-\nhersage am wichtigsten sind.\n4.3 Benchmarking und Vergleich\nUm die Effektivit ¨at der verschiedenen Methoden zu bewerten, wird ein Benchmarking-\nAnsatz verfolgt. Dazu werden konsistente Metriken wie die Vorhersagegenauig-\nkeit, die Feature-Wichtigkeitsrankings und die Interpretierbarkeit der Modelle']</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>It is about love</t>
-        </is>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>